<commit_message>
Changes made following review 1
</commit_message>
<xml_diff>
--- a/src/Database/DataModel_v1.xlsx
+++ b/src/Database/DataModel_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\andrew\vector-atlas\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D315358-658F-4927-BBA2-DCA3D5245ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D154F7-3965-4599-8CF5-F52155F38D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" firstSheet="3" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bionomics" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="533" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="217">
   <si>
     <t>Column name</t>
   </si>
@@ -1031,8 +1031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,19 +1105,31 @@
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1552,7 +1564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C026395D-A46F-4645-B157-59F1158E3B7F}">
   <dimension ref="B2:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated the data model with Antionette's notes
</commit_message>
<xml_diff>
--- a/src/Database/DataModel_v1.xlsx
+++ b/src/Database/DataModel_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\andrew\vector-atlas\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69D154F7-3965-4599-8CF5-F52155F38D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA603E43-0AFE-4074-AC2E-925501221461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bionomics" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="217">
   <si>
     <t>Column name</t>
   </si>
@@ -694,17 +694,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -718,17 +711,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -740,17 +728,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1031,7 +1016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10:D10"/>
     </sheetView>
   </sheetViews>
@@ -1932,8 +1917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293BF017-667C-4E48-9509-5459E3DD1428}">
   <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1987,7 +1972,12 @@
       <c r="B6" t="s">
         <v>179</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
@@ -2029,7 +2019,7 @@
   <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2116,13 +2106,23 @@
       <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -2139,7 +2139,9 @@
       <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -2153,7 +2155,12 @@
       <c r="B14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>250</v>
+      </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
@@ -2551,7 +2558,7 @@
   <dimension ref="B2:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:D29"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2668,7 +2675,9 @@
       <c r="B12" t="s">
         <v>61</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -2822,7 +2831,7 @@
   <dimension ref="B2:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2979,37 +2988,49 @@
       <c r="B16" t="s">
         <v>88</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>89</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>90</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>92</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>93</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">

</xml_diff>

<commit_message>
Added migration for base bionomics type
</commit_message>
<xml_diff>
--- a/src/Database/DataModel_v1.xlsx
+++ b/src/Database/DataModel_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\andrew\vector-atlas\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA603E43-0AFE-4074-AC2E-925501221461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CB874D-0845-47A2-94D5-C53B8C6FF1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" firstSheet="3" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bionomics" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="219">
   <si>
     <t>Column name</t>
   </si>
@@ -688,6 +688,12 @@
   </si>
   <si>
     <t>Endo_Exophiliy_Bionomics</t>
+  </si>
+  <si>
+    <t>Tabled?</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -1014,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F33"/>
+  <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1034,10 @@
     <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>217</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1045,7 +1054,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -1059,7 +1071,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -1070,7 +1082,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -1078,7 +1093,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
@@ -1086,7 +1104,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
@@ -1094,7 +1115,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
@@ -1105,7 +1129,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -1116,7 +1143,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -1127,7 +1154,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
       <c r="B12" t="s">
         <v>37</v>
       </c>
@@ -1135,7 +1165,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>218</v>
+      </c>
       <c r="B13" t="s">
         <v>38</v>
       </c>
@@ -1146,7 +1179,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
       <c r="B14" t="s">
         <v>39</v>
       </c>
@@ -1157,7 +1193,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>218</v>
+      </c>
       <c r="B15" t="s">
         <v>40</v>
       </c>
@@ -1165,7 +1204,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>218</v>
+      </c>
       <c r="B16" t="s">
         <v>41</v>
       </c>
@@ -1173,7 +1215,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>218</v>
+      </c>
       <c r="B17" t="s">
         <v>42</v>
       </c>
@@ -1181,7 +1226,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
       <c r="B18" t="s">
         <v>43</v>
       </c>
@@ -1189,7 +1237,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>218</v>
+      </c>
       <c r="B19" t="s">
         <v>44</v>
       </c>
@@ -1200,7 +1251,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>218</v>
+      </c>
       <c r="B20" t="s">
         <v>45</v>
       </c>
@@ -1211,7 +1265,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>218</v>
+      </c>
       <c r="B21" t="s">
         <v>46</v>
       </c>
@@ -1222,7 +1279,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>181</v>
       </c>
@@ -1233,7 +1290,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>218</v>
+      </c>
       <c r="B23" t="s">
         <v>50</v>
       </c>
@@ -1244,7 +1304,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>218</v>
+      </c>
       <c r="B24" t="s">
         <v>51</v>
       </c>
@@ -1255,7 +1318,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>218</v>
+      </c>
       <c r="B25" t="s">
         <v>164</v>
       </c>
@@ -1266,7 +1332,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>218</v>
+      </c>
       <c r="B26" t="s">
         <v>165</v>
       </c>
@@ -1277,7 +1346,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>203</v>
       </c>
@@ -1285,7 +1354,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>204</v>
       </c>
@@ -1293,7 +1362,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>205</v>
       </c>
@@ -1301,7 +1370,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>209</v>
       </c>
@@ -1309,7 +1378,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>210</v>
       </c>
@@ -1317,7 +1386,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>212</v>
       </c>
@@ -1917,7 +1986,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293BF017-667C-4E48-9509-5459E3DD1428}">
   <dimension ref="B2:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added Reference and SIte entities, linked to Bionomics, with migration
</commit_message>
<xml_diff>
--- a/src/Database/DataModel_v1.xlsx
+++ b/src/Database/DataModel_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\andrew\vector-atlas\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01CB874D-0845-47A2-94D5-C53B8C6FF1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667DB938-B1C8-414A-928D-ED86E28F7008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bionomics" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="220">
   <si>
     <t>Column name</t>
   </si>
@@ -694,6 +694,9 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Tabled</t>
   </si>
 </sst>
 </file>
@@ -1023,7 +1026,7 @@
   <dimension ref="A2:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1072,6 +1075,9 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -1144,6 +1150,9 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -2085,10 +2094,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978D90C2-152C-488B-A7D2-35719C771FB5}">
-  <dimension ref="B2:F25"/>
+  <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2099,7 +2108,10 @@
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2116,7 +2128,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2127,7 +2142,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
       <c r="B5" t="s">
         <v>24</v>
       </c>
@@ -2138,7 +2156,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
       <c r="B6" t="s">
         <v>25</v>
       </c>
@@ -2149,7 +2170,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
       <c r="B7" t="s">
         <v>26</v>
       </c>
@@ -2160,7 +2184,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
       <c r="B8" t="s">
         <v>27</v>
       </c>
@@ -2171,7 +2198,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
       <c r="B9" t="s">
         <v>31</v>
       </c>
@@ -2182,7 +2212,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
       <c r="B10" t="s">
         <v>32</v>
       </c>
@@ -2193,7 +2226,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
       <c r="B11" t="s">
         <v>33</v>
       </c>
@@ -2204,7 +2240,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
       <c r="B12" t="s">
         <v>34</v>
       </c>
@@ -2212,7 +2251,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>218</v>
+      </c>
       <c r="B13" t="s">
         <v>35</v>
       </c>
@@ -2220,7 +2262,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
       <c r="B14" t="s">
         <v>36</v>
       </c>
@@ -2231,7 +2276,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>218</v>
+      </c>
       <c r="B15" t="s">
         <v>168</v>
       </c>
@@ -2242,7 +2290,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>218</v>
+      </c>
       <c r="B16" t="s">
         <v>169</v>
       </c>
@@ -2253,7 +2304,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>218</v>
+      </c>
       <c r="B17" t="s">
         <v>170</v>
       </c>
@@ -2264,7 +2318,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
       <c r="B18" t="s">
         <v>171</v>
       </c>
@@ -2272,7 +2329,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>218</v>
+      </c>
       <c r="B19" t="s">
         <v>172</v>
       </c>
@@ -2280,7 +2340,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>218</v>
+      </c>
       <c r="B20" t="s">
         <v>173</v>
       </c>
@@ -2291,7 +2354,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>218</v>
+      </c>
       <c r="B21" t="s">
         <v>174</v>
       </c>
@@ -2299,7 +2365,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>218</v>
+      </c>
       <c r="B22" t="s">
         <v>175</v>
       </c>
@@ -2307,7 +2376,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>218</v>
+      </c>
       <c r="B23" t="s">
         <v>176</v>
       </c>
@@ -2318,7 +2390,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>218</v>
+      </c>
       <c r="B24" t="s">
         <v>177</v>
       </c>
@@ -2326,7 +2401,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>218</v>
+      </c>
       <c r="B25" t="s">
         <v>178</v>
       </c>
@@ -2341,10 +2419,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{210D81B4-7A46-43E5-8A09-EDA7446CCEBF}">
-  <dimension ref="B2:E11"/>
+  <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2355,7 +2433,10 @@
     <col min="5" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2369,7 +2450,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2383,7 +2467,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
       <c r="B5" t="s">
         <v>12</v>
       </c>
@@ -2394,7 +2481,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -2405,7 +2495,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
@@ -2416,7 +2509,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
@@ -2424,7 +2520,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -2432,7 +2531,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
       <c r="B10" t="s">
         <v>166</v>
       </c>
@@ -2443,7 +2545,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
       <c r="B11" t="s">
         <v>167</v>
       </c>

</xml_diff>

<commit_message>
Added species and biology entities
</commit_message>
<xml_diff>
--- a/src/Database/DataModel_v1.xlsx
+++ b/src/Database/DataModel_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\andrew\vector-atlas\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667DB938-B1C8-414A-928D-ED86E28F7008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC22FFF-06AF-47D7-B52C-AC649B3A5394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bionomics" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="603" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="220">
   <si>
     <t>Column name</t>
   </si>
@@ -1025,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,6 +1289,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>218</v>
+      </c>
       <c r="B22" t="s">
         <v>181</v>
       </c>
@@ -1627,7 +1630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C026395D-A46F-4645-B157-59F1158E3B7F}">
   <dimension ref="B2:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -1993,10 +1996,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293BF017-667C-4E48-9509-5459E3DD1428}">
-  <dimension ref="B2:E9"/>
+  <dimension ref="A2:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2004,7 +2007,10 @@
     <col min="2" max="5" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2018,7 +2024,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2032,7 +2041,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
       <c r="B5" t="s">
         <v>47</v>
       </c>
@@ -2046,7 +2058,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
       <c r="B6" t="s">
         <v>179</v>
       </c>
@@ -2057,7 +2072,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
       <c r="B7" t="s">
         <v>49</v>
       </c>
@@ -2065,7 +2083,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
       <c r="B8" t="s">
         <v>180</v>
       </c>
@@ -2076,7 +2097,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
       <c r="B9" t="s">
         <v>48</v>
       </c>
@@ -2563,10 +2587,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B965F3-143D-479A-9288-34A19C721D8C}">
-  <dimension ref="B2:E16"/>
+  <dimension ref="A2:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2577,7 +2601,7 @@
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2591,7 +2615,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2605,7 +2632,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
       <c r="B5" t="s">
         <v>94</v>
       </c>
@@ -2619,7 +2649,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
       <c r="B6" t="s">
         <v>96</v>
       </c>
@@ -2630,7 +2663,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
       <c r="B7" t="s">
         <v>97</v>
       </c>
@@ -2641,7 +2677,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
       <c r="B8" t="s">
         <v>98</v>
       </c>
@@ -2652,7 +2691,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
       <c r="B9" t="s">
         <v>99</v>
       </c>
@@ -2663,7 +2705,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>52</v>
       </c>
@@ -2671,7 +2713,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>53</v>
       </c>
@@ -2679,7 +2721,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>54</v>
       </c>
@@ -2687,7 +2729,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>56</v>
       </c>
@@ -2695,7 +2737,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>57</v>
       </c>
@@ -2703,7 +2745,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>58</v>
       </c>
@@ -2711,7 +2753,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>95</v>
       </c>

</xml_diff>

<commit_message>
Added foreign keys to parent entities
</commit_message>
<xml_diff>
--- a/src/Database/DataModel_v1.xlsx
+++ b/src/Database/DataModel_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\andrew\vector-atlas\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC22FFF-06AF-47D7-B52C-AC649B3A5394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{D54E0AF4-43CC-4B79-ABC3-C7AA0A4D1206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" firstSheet="3" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bionomics" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="220">
   <si>
     <t>Column name</t>
   </si>
@@ -1422,10 +1422,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99AF858D-8BD8-46A2-B904-D834D566FA4E}">
-  <dimension ref="B2:E22"/>
+  <dimension ref="A2:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E4"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,7 +1434,10 @@
     <col min="3" max="5" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1448,7 +1451,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -1462,7 +1468,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
       <c r="B5" t="s">
         <v>94</v>
       </c>
@@ -1476,7 +1485,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
       <c r="B6" t="s">
         <v>148</v>
       </c>
@@ -1487,7 +1499,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
       <c r="B7" t="s">
         <v>149</v>
       </c>
@@ -1495,7 +1510,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
       <c r="B8" t="s">
         <v>150</v>
       </c>
@@ -1503,7 +1521,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
       <c r="B9" t="s">
         <v>151</v>
       </c>
@@ -1511,7 +1532,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
       <c r="B10" t="s">
         <v>152</v>
       </c>
@@ -1519,7 +1543,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
       <c r="B11" t="s">
         <v>153</v>
       </c>
@@ -1527,7 +1554,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
       <c r="B12" t="s">
         <v>154</v>
       </c>
@@ -1535,7 +1565,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>218</v>
+      </c>
       <c r="B13" t="s">
         <v>155</v>
       </c>
@@ -1543,7 +1576,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
       <c r="B14" t="s">
         <v>156</v>
       </c>
@@ -1551,7 +1587,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>218</v>
+      </c>
       <c r="B15" t="s">
         <v>157</v>
       </c>
@@ -1559,7 +1598,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>218</v>
+      </c>
       <c r="B16" t="s">
         <v>158</v>
       </c>
@@ -1567,7 +1609,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>218</v>
+      </c>
       <c r="B17" t="s">
         <v>159</v>
       </c>
@@ -1575,7 +1620,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
       <c r="B18" t="s">
         <v>160</v>
       </c>
@@ -1583,7 +1631,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>218</v>
+      </c>
       <c r="B19" t="s">
         <v>161</v>
       </c>
@@ -1591,7 +1642,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>218</v>
+      </c>
       <c r="B20" t="s">
         <v>162</v>
       </c>
@@ -1599,7 +1653,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>218</v>
+      </c>
       <c r="B21" t="s">
         <v>163</v>
       </c>
@@ -1610,7 +1667,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>218</v>
+      </c>
       <c r="B22" t="s">
         <v>95</v>
       </c>
@@ -1628,10 +1688,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C026395D-A46F-4645-B157-59F1158E3B7F}">
-  <dimension ref="B2:E16"/>
+  <dimension ref="A2:E16"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,7 +1699,10 @@
     <col min="2" max="5" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1653,7 +1716,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -1667,7 +1733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>16</v>
       </c>
@@ -1678,7 +1744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>22</v>
       </c>
@@ -1689,7 +1755,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
       <c r="B7" t="s">
         <v>40</v>
       </c>
@@ -1697,7 +1766,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
       <c r="B8" t="s">
         <v>41</v>
       </c>
@@ -1705,7 +1777,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
       <c r="B9" t="s">
         <v>42</v>
       </c>
@@ -1713,7 +1788,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
       <c r="B10" t="s">
         <v>43</v>
       </c>
@@ -1721,7 +1799,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>181</v>
       </c>
@@ -1732,7 +1810,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>197</v>
       </c>
@@ -1743,7 +1821,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>218</v>
+      </c>
       <c r="B13" t="s">
         <v>199</v>
       </c>
@@ -1757,7 +1838,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
       <c r="B14" t="s">
         <v>200</v>
       </c>
@@ -1768,7 +1852,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>218</v>
+      </c>
       <c r="B15" t="s">
         <v>201</v>
       </c>
@@ -1779,7 +1866,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>218</v>
+      </c>
       <c r="B16" t="s">
         <v>202</v>
       </c>
@@ -1799,8 +1889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE8B3D8-A9ED-46BF-98BF-521094278ACE}">
   <dimension ref="B2:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2589,8 +2679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55B965F3-143D-479A-9288-34A19C721D8C}">
   <dimension ref="A2:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2706,6 +2796,9 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
       <c r="B10" t="s">
         <v>52</v>
       </c>
@@ -2714,6 +2807,9 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
       <c r="B11" t="s">
         <v>53</v>
       </c>
@@ -2722,6 +2818,9 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
       <c r="B12" t="s">
         <v>54</v>
       </c>
@@ -2730,6 +2829,9 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>218</v>
+      </c>
       <c r="B13" t="s">
         <v>56</v>
       </c>
@@ -2738,6 +2840,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
       <c r="B14" t="s">
         <v>57</v>
       </c>
@@ -2746,6 +2851,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>218</v>
+      </c>
       <c r="B15" t="s">
         <v>58</v>
       </c>
@@ -2754,6 +2862,9 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>218</v>
+      </c>
       <c r="B16" t="s">
         <v>95</v>
       </c>
@@ -2771,10 +2882,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4075B4B3-18B2-49EF-A8B3-FB90FBA5AEDC}">
-  <dimension ref="B2:E29"/>
+  <dimension ref="A2:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2785,7 +2896,10 @@
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2799,7 +2913,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -2813,7 +2930,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
       <c r="B5" t="s">
         <v>94</v>
       </c>
@@ -2827,7 +2947,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
       <c r="B6" t="s">
         <v>96</v>
       </c>
@@ -2838,7 +2961,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
       <c r="B7" t="s">
         <v>97</v>
       </c>
@@ -2849,7 +2975,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
       <c r="B8" t="s">
         <v>98</v>
       </c>
@@ -2860,7 +2989,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
       <c r="B9" t="s">
         <v>99</v>
       </c>
@@ -2871,7 +3003,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
       <c r="B10" t="s">
         <v>59</v>
       </c>
@@ -2879,7 +3014,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
       <c r="B11" t="s">
         <v>60</v>
       </c>
@@ -2887,7 +3025,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
       <c r="B12" t="s">
         <v>61</v>
       </c>
@@ -2895,7 +3036,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>218</v>
+      </c>
       <c r="B13" t="s">
         <v>62</v>
       </c>
@@ -2903,7 +3047,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
       <c r="B14" t="s">
         <v>63</v>
       </c>
@@ -2911,7 +3058,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>218</v>
+      </c>
       <c r="B15" t="s">
         <v>65</v>
       </c>
@@ -2919,7 +3069,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>218</v>
+      </c>
       <c r="B16" t="s">
         <v>64</v>
       </c>
@@ -2927,15 +3080,21 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>218</v>
+      </c>
       <c r="B17" t="s">
         <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
       <c r="B18" t="s">
         <v>67</v>
       </c>
@@ -2943,7 +3102,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>218</v>
+      </c>
       <c r="B19" t="s">
         <v>68</v>
       </c>
@@ -2951,7 +3113,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>218</v>
+      </c>
       <c r="B20" t="s">
         <v>69</v>
       </c>
@@ -2959,7 +3124,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>218</v>
+      </c>
       <c r="B21" t="s">
         <v>70</v>
       </c>
@@ -2967,7 +3135,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>218</v>
+      </c>
       <c r="B22" t="s">
         <v>71</v>
       </c>
@@ -2975,7 +3146,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>218</v>
+      </c>
       <c r="B23" t="s">
         <v>72</v>
       </c>
@@ -2983,7 +3157,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>218</v>
+      </c>
       <c r="B24" t="s">
         <v>73</v>
       </c>
@@ -2991,7 +3168,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>218</v>
+      </c>
       <c r="B25" t="s">
         <v>74</v>
       </c>
@@ -2999,7 +3179,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>218</v>
+      </c>
       <c r="B26" t="s">
         <v>75</v>
       </c>
@@ -3007,7 +3190,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>218</v>
+      </c>
       <c r="B27" t="s">
         <v>76</v>
       </c>
@@ -3018,7 +3204,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>218</v>
+      </c>
       <c r="B28" t="s">
         <v>77</v>
       </c>
@@ -3026,7 +3215,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>218</v>
+      </c>
       <c r="B29" t="s">
         <v>95</v>
       </c>
@@ -3044,10 +3236,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9ACCAA4-81D7-40B1-B57D-E3ED0B555CFE}">
-  <dimension ref="B2:E22"/>
+  <dimension ref="A2:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3057,7 +3249,10 @@
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3071,7 +3266,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -3085,7 +3283,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
       <c r="B5" t="s">
         <v>94</v>
       </c>
@@ -3099,7 +3300,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
       <c r="B6" t="s">
         <v>78</v>
       </c>
@@ -3110,7 +3314,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
       <c r="B7" t="s">
         <v>79</v>
       </c>
@@ -3118,7 +3325,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
       <c r="B8" t="s">
         <v>80</v>
       </c>
@@ -3129,7 +3339,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
       <c r="B9" t="s">
         <v>81</v>
       </c>
@@ -3137,7 +3350,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
       <c r="B10" t="s">
         <v>82</v>
       </c>
@@ -3148,7 +3364,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
       <c r="B11" t="s">
         <v>83</v>
       </c>
@@ -3159,7 +3378,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
       <c r="B12" t="s">
         <v>84</v>
       </c>
@@ -3170,7 +3392,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>218</v>
+      </c>
       <c r="B13" t="s">
         <v>85</v>
       </c>
@@ -3181,7 +3406,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
       <c r="B14" t="s">
         <v>86</v>
       </c>
@@ -3189,7 +3417,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>218</v>
+      </c>
       <c r="B15" t="s">
         <v>87</v>
       </c>
@@ -3200,7 +3431,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>218</v>
+      </c>
       <c r="B16" t="s">
         <v>88</v>
       </c>
@@ -3208,7 +3442,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>218</v>
+      </c>
       <c r="B17" t="s">
         <v>89</v>
       </c>
@@ -3216,7 +3453,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
       <c r="B18" t="s">
         <v>90</v>
       </c>
@@ -3224,7 +3464,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>218</v>
+      </c>
       <c r="B19" t="s">
         <v>91</v>
       </c>
@@ -3232,7 +3475,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>92</v>
       </c>
@@ -3240,7 +3483,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>93</v>
       </c>
@@ -3248,7 +3491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>95</v>
       </c>
@@ -3266,10 +3509,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C97208F-F025-401B-A51A-98116DE80443}">
-  <dimension ref="B2:E30"/>
+  <dimension ref="A2:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30:D30"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3280,7 +3523,10 @@
     <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3294,7 +3540,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -3308,7 +3557,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
       <c r="B5" t="s">
         <v>94</v>
       </c>
@@ -3322,7 +3574,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
       <c r="B6" t="s">
         <v>100</v>
       </c>
@@ -3333,7 +3588,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
       <c r="B7" t="s">
         <v>101</v>
       </c>
@@ -3341,7 +3599,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
       <c r="B8" t="s">
         <v>102</v>
       </c>
@@ -3349,7 +3610,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
       <c r="B9" t="s">
         <v>103</v>
       </c>
@@ -3357,7 +3621,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
       <c r="B10" t="s">
         <v>123</v>
       </c>
@@ -3368,7 +3635,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
       <c r="B11" t="s">
         <v>104</v>
       </c>
@@ -3376,7 +3646,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
       <c r="B12" t="s">
         <v>105</v>
       </c>
@@ -3384,7 +3657,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>218</v>
+      </c>
       <c r="B13" t="s">
         <v>106</v>
       </c>
@@ -3392,7 +3668,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
       <c r="B14" t="s">
         <v>107</v>
       </c>
@@ -3403,7 +3682,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>218</v>
+      </c>
       <c r="B15" t="s">
         <v>108</v>
       </c>
@@ -3414,7 +3696,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>218</v>
+      </c>
       <c r="B16" t="s">
         <v>109</v>
       </c>
@@ -3425,7 +3710,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>218</v>
+      </c>
       <c r="B17" t="s">
         <v>110</v>
       </c>
@@ -3436,7 +3724,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
       <c r="B18" t="s">
         <v>111</v>
       </c>
@@ -3444,7 +3735,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>218</v>
+      </c>
       <c r="B19" t="s">
         <v>112</v>
       </c>
@@ -3452,7 +3746,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>218</v>
+      </c>
       <c r="B20" t="s">
         <v>113</v>
       </c>
@@ -3460,7 +3757,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>218</v>
+      </c>
       <c r="B21" t="s">
         <v>114</v>
       </c>
@@ -3471,7 +3771,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>218</v>
+      </c>
       <c r="B22" t="s">
         <v>115</v>
       </c>
@@ -3482,7 +3785,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>218</v>
+      </c>
       <c r="B23" t="s">
         <v>116</v>
       </c>
@@ -3493,7 +3799,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>218</v>
+      </c>
       <c r="B24" t="s">
         <v>117</v>
       </c>
@@ -3504,7 +3813,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>218</v>
+      </c>
       <c r="B25" t="s">
         <v>118</v>
       </c>
@@ -3515,7 +3827,10 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>218</v>
+      </c>
       <c r="B26" t="s">
         <v>119</v>
       </c>
@@ -3523,7 +3838,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>218</v>
+      </c>
       <c r="B27" t="s">
         <v>120</v>
       </c>
@@ -3531,7 +3849,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>218</v>
+      </c>
       <c r="B28" t="s">
         <v>121</v>
       </c>
@@ -3539,7 +3860,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>218</v>
+      </c>
       <c r="B29" t="s">
         <v>122</v>
       </c>
@@ -3550,7 +3874,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>218</v>
+      </c>
       <c r="B30" t="s">
         <v>95</v>
       </c>
@@ -3568,10 +3895,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F87B62-CB96-4093-8E9A-05046B02A68C}">
-  <dimension ref="B2:E17"/>
+  <dimension ref="A2:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:D17"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3580,7 +3907,10 @@
     <col min="3" max="5" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3594,7 +3924,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -3608,7 +3941,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
       <c r="B5" t="s">
         <v>94</v>
       </c>
@@ -3622,7 +3958,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
       <c r="B6" t="s">
         <v>125</v>
       </c>
@@ -3630,7 +3969,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
       <c r="B7" t="s">
         <v>124</v>
       </c>
@@ -3641,7 +3983,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
       <c r="B8" t="s">
         <v>126</v>
       </c>
@@ -3649,7 +3994,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
       <c r="B9" t="s">
         <v>127</v>
       </c>
@@ -3657,7 +4005,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
       <c r="B10" t="s">
         <v>128</v>
       </c>
@@ -3665,7 +4016,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
       <c r="B11" t="s">
         <v>129</v>
       </c>
@@ -3673,7 +4027,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
       <c r="B12" t="s">
         <v>130</v>
       </c>
@@ -3684,7 +4041,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>218</v>
+      </c>
       <c r="B13" t="s">
         <v>131</v>
       </c>
@@ -3692,7 +4052,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
       <c r="B14" t="s">
         <v>132</v>
       </c>
@@ -3700,7 +4063,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>218</v>
+      </c>
       <c r="B15" t="s">
         <v>133</v>
       </c>
@@ -3708,7 +4074,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>218</v>
+      </c>
       <c r="B16" t="s">
         <v>134</v>
       </c>
@@ -3719,7 +4088,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>218</v>
+      </c>
       <c r="B17" t="s">
         <v>95</v>
       </c>
@@ -3737,10 +4109,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98790CFE-4FCB-4540-96DB-BF7001C67FC5}">
-  <dimension ref="B2:E21"/>
+  <dimension ref="A2:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3749,7 +4121,10 @@
     <col min="3" max="5" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -3763,7 +4138,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
@@ -3777,7 +4155,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
       <c r="B5" t="s">
         <v>94</v>
       </c>
@@ -3791,7 +4172,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>125</v>
       </c>
@@ -3799,7 +4180,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>135</v>
       </c>
@@ -3807,7 +4188,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>136</v>
       </c>
@@ -3815,7 +4196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>137</v>
       </c>
@@ -3823,7 +4204,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>138</v>
       </c>
@@ -3831,7 +4212,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>129</v>
       </c>
@@ -3839,7 +4220,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>139</v>
       </c>
@@ -3847,7 +4228,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>140</v>
       </c>
@@ -3855,7 +4236,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>141</v>
       </c>
@@ -3863,7 +4244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>142</v>
       </c>
@@ -3871,7 +4252,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>143</v>
       </c>

</xml_diff>

<commit_message>
Environment and bionomics updates
</commit_message>
<xml_diff>
--- a/src/Database/DataModel_v1.xlsx
+++ b/src/Database/DataModel_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\andrew\vector-atlas\src\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\sanc\vector-atlas\src\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A314D705-2B6E-44AB-B3DD-631C4866ABA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE45A86-4EEE-4BE7-B3CD-8108DAAB1D67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="864" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19725" yWindow="-21720" windowWidth="38640" windowHeight="21240" tabRatio="864" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bionomics" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <sheet name="Occurrence" sheetId="11" r:id="rId11"/>
     <sheet name="Sample" sheetId="13" r:id="rId12"/>
     <sheet name="Species" sheetId="12" r:id="rId13"/>
+    <sheet name="Environment" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="239">
   <si>
     <t>Column name</t>
   </si>
@@ -697,6 +698,63 @@
   </si>
   <si>
     <t>Tabled</t>
+  </si>
+  <si>
+    <t>study_sampling_design</t>
+  </si>
+  <si>
+    <t>itn_use</t>
+  </si>
+  <si>
+    <t>species_notes</t>
+  </si>
+  <si>
+    <t>roof</t>
+  </si>
+  <si>
+    <t>walls</t>
+  </si>
+  <si>
+    <t>house_screening</t>
+  </si>
+  <si>
+    <t>open_eaves</t>
+  </si>
+  <si>
+    <t>cooking</t>
+  </si>
+  <si>
+    <t>housing_notes</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>outdoor_activities_night</t>
+  </si>
+  <si>
+    <t>sleeping_outdoors</t>
+  </si>
+  <si>
+    <t>community_notes</t>
+  </si>
+  <si>
+    <t>farming</t>
+  </si>
+  <si>
+    <t>farming_notes</t>
+  </si>
+  <si>
+    <t>livestock</t>
+  </si>
+  <si>
+    <t>livestock_notes</t>
+  </si>
+  <si>
+    <t>local_plants</t>
+  </si>
+  <si>
+    <t>Booleam</t>
   </si>
 </sst>
 </file>
@@ -1023,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:F33"/>
+  <dimension ref="A2:F35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,14 +1169,14 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>218</v>
-      </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>220</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1126,13 +1184,10 @@
         <v>218</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9">
-        <v>50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1140,7 +1195,7 @@
         <v>218</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -1154,13 +1209,13 @@
         <v>218</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D11">
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1168,10 +1223,13 @@
         <v>218</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>9</v>
+        <v>23</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1179,7 +1237,7 @@
         <v>218</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>221</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -1193,13 +1251,10 @@
         <v>218</v>
       </c>
       <c r="B14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>250</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1207,10 +1262,13 @@
         <v>218</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>250</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1218,10 +1276,13 @@
         <v>218</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1229,7 +1290,7 @@
         <v>218</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C17" t="s">
         <v>8</v>
@@ -1240,7 +1301,7 @@
         <v>218</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -1251,13 +1312,10 @@
         <v>218</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1265,13 +1323,10 @@
         <v>218</v>
       </c>
       <c r="B20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1279,13 +1334,13 @@
         <v>218</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21">
-        <v>250</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,13 +1348,13 @@
         <v>218</v>
       </c>
       <c r="B22" t="s">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="C22" t="s">
-        <v>182</v>
-      </c>
-      <c r="E22" t="s">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1307,7 +1362,7 @@
         <v>218</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -1321,13 +1376,13 @@
         <v>218</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>181</v>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
-      </c>
-      <c r="D24">
-        <v>250</v>
+        <v>182</v>
+      </c>
+      <c r="E24" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1335,13 +1390,13 @@
         <v>218</v>
       </c>
       <c r="B25" t="s">
-        <v>164</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25">
-        <v>50</v>
+        <v>250</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1349,68 +1404,96 @@
         <v>218</v>
       </c>
       <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>218</v>
+      </c>
+      <c r="B27" t="s">
+        <v>164</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>218</v>
+      </c>
+      <c r="B28" t="s">
         <v>165</v>
       </c>
-      <c r="C26" t="s">
-        <v>4</v>
-      </c>
-      <c r="D26">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>203</v>
-      </c>
-      <c r="C27" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>204</v>
-      </c>
       <c r="C28" t="s">
-        <v>207</v>
+        <v>4</v>
+      </c>
+      <c r="D28">
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C29" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C30" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="C31" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C32" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>210</v>
+      </c>
+      <c r="C33" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>212</v>
+      </c>
+      <c r="C34" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>214</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>216</v>
       </c>
     </row>
@@ -2086,10 +2169,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293BF017-667C-4E48-9509-5459E3DD1428}">
-  <dimension ref="A2:E9"/>
+  <dimension ref="A2:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="W39" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2201,6 +2284,256 @@
         <v>50</v>
       </c>
     </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" t="s">
+        <v>222</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5735511B-D5A9-4985-BBB5-983F1E7592B7}">
+  <dimension ref="A2:E18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="W32" sqref="W32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="5" width="15.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>218</v>
+      </c>
+      <c r="B4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B5" t="s">
+        <v>224</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>218</v>
+      </c>
+      <c r="B6" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B9" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>218</v>
+      </c>
+      <c r="B10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" t="s">
+        <v>230</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>218</v>
+      </c>
+      <c r="B12" t="s">
+        <v>231</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>218</v>
+      </c>
+      <c r="B13" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>218</v>
+      </c>
+      <c r="B14" t="s">
+        <v>233</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>218</v>
+      </c>
+      <c r="B15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B16" t="s">
+        <v>235</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>218</v>
+      </c>
+      <c r="B17" t="s">
+        <v>236</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>218</v>
+      </c>
+      <c r="B18" t="s">
+        <v>237</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2210,8 +2543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978D90C2-152C-488B-A7D2-35719C771FB5}">
   <dimension ref="A2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2884,8 +3217,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4075B4B3-18B2-49EF-A8B3-FB90FBA5AEDC}">
   <dimension ref="A2:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>